<commit_message>
Update edited session - 2025-10-20T09:08:23.746Z - Cache Bust ID: 1760951303746zvj6daf7n
</commit_message>
<xml_diff>
--- a/log_history/Y4_B2526_General_Surgery_scanner1760947731738_412de898fa38de7e284b58047ef9f3c3397f8d8f5931e4595a3fdbe4844ec332.xlsx
+++ b/log_history/Y4_B2526_General_Surgery_scanner1760947731738_412de898fa38de7e284b58047ef9f3c3397f8d8f5931e4595a3fdbe4844ec332.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Scanner" sheetId="1" r:id="rId1"/>
+    <sheet name="Session" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F101"/>
+  <dimension ref="A1:F100"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1464,7 +1464,7 @@
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>202089</v>
+        <v>211167</v>
       </c>
       <c r="B54" t="str">
         <v>General Surgery</v>
@@ -1473,7 +1473,7 @@
         <v>20/10/2025</v>
       </c>
       <c r="D54" t="str">
-        <v>11:15:20</v>
+        <v>11:15:26</v>
       </c>
       <c r="E54" t="str">
         <v>Manual</v>
@@ -1484,7 +1484,7 @@
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>211167</v>
+        <v>211118</v>
       </c>
       <c r="B55" t="str">
         <v>General Surgery</v>
@@ -1493,7 +1493,7 @@
         <v>20/10/2025</v>
       </c>
       <c r="D55" t="str">
-        <v>11:15:26</v>
+        <v>11:15:31</v>
       </c>
       <c r="E55" t="str">
         <v>Manual</v>
@@ -1504,7 +1504,7 @@
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>211118</v>
+        <v>211146</v>
       </c>
       <c r="B56" t="str">
         <v>General Surgery</v>
@@ -1513,7 +1513,7 @@
         <v>20/10/2025</v>
       </c>
       <c r="D56" t="str">
-        <v>11:15:31</v>
+        <v>11:15:38</v>
       </c>
       <c r="E56" t="str">
         <v>Manual</v>
@@ -1524,7 +1524,7 @@
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>211146</v>
+        <v>211092</v>
       </c>
       <c r="B57" t="str">
         <v>General Surgery</v>
@@ -1533,7 +1533,7 @@
         <v>20/10/2025</v>
       </c>
       <c r="D57" t="str">
-        <v>11:15:38</v>
+        <v>11:15:43</v>
       </c>
       <c r="E57" t="str">
         <v>Manual</v>
@@ -1544,7 +1544,7 @@
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>211092</v>
+        <v>201795</v>
       </c>
       <c r="B58" t="str">
         <v>General Surgery</v>
@@ -1553,7 +1553,7 @@
         <v>20/10/2025</v>
       </c>
       <c r="D58" t="str">
-        <v>11:15:43</v>
+        <v>11:16:01</v>
       </c>
       <c r="E58" t="str">
         <v>Manual</v>
@@ -1564,7 +1564,7 @@
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>201795</v>
+        <v>211174</v>
       </c>
       <c r="B59" t="str">
         <v>General Surgery</v>
@@ -1573,7 +1573,7 @@
         <v>20/10/2025</v>
       </c>
       <c r="D59" t="str">
-        <v>11:16:01</v>
+        <v>11:16:16</v>
       </c>
       <c r="E59" t="str">
         <v>Manual</v>
@@ -1584,7 +1584,7 @@
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>211174</v>
+        <v>211086</v>
       </c>
       <c r="B60" t="str">
         <v>General Surgery</v>
@@ -1593,7 +1593,7 @@
         <v>20/10/2025</v>
       </c>
       <c r="D60" t="str">
-        <v>11:16:16</v>
+        <v>11:16:22</v>
       </c>
       <c r="E60" t="str">
         <v>Manual</v>
@@ -1604,7 +1604,7 @@
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>211086</v>
+        <v>211175</v>
       </c>
       <c r="B61" t="str">
         <v>General Surgery</v>
@@ -1613,7 +1613,7 @@
         <v>20/10/2025</v>
       </c>
       <c r="D61" t="str">
-        <v>11:16:22</v>
+        <v>11:16:32</v>
       </c>
       <c r="E61" t="str">
         <v>Manual</v>
@@ -1624,7 +1624,7 @@
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>211175</v>
+        <v>202041</v>
       </c>
       <c r="B62" t="str">
         <v>General Surgery</v>
@@ -1633,7 +1633,7 @@
         <v>20/10/2025</v>
       </c>
       <c r="D62" t="str">
-        <v>11:16:32</v>
+        <v>11:16:42</v>
       </c>
       <c r="E62" t="str">
         <v>Manual</v>
@@ -1644,7 +1644,7 @@
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>202041</v>
+        <v>210923</v>
       </c>
       <c r="B63" t="str">
         <v>General Surgery</v>
@@ -1653,7 +1653,7 @@
         <v>20/10/2025</v>
       </c>
       <c r="D63" t="str">
-        <v>11:16:42</v>
+        <v>11:16:58</v>
       </c>
       <c r="E63" t="str">
         <v>Manual</v>
@@ -1664,7 +1664,7 @@
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>210923</v>
+        <v>202162</v>
       </c>
       <c r="B64" t="str">
         <v>General Surgery</v>
@@ -1673,7 +1673,7 @@
         <v>20/10/2025</v>
       </c>
       <c r="D64" t="str">
-        <v>11:16:58</v>
+        <v>11:17:14</v>
       </c>
       <c r="E64" t="str">
         <v>Manual</v>
@@ -1684,7 +1684,7 @@
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>202162</v>
+        <v>211102</v>
       </c>
       <c r="B65" t="str">
         <v>General Surgery</v>
@@ -1693,7 +1693,7 @@
         <v>20/10/2025</v>
       </c>
       <c r="D65" t="str">
-        <v>11:17:14</v>
+        <v>11:17:22</v>
       </c>
       <c r="E65" t="str">
         <v>Manual</v>
@@ -1704,7 +1704,7 @@
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>211102</v>
+        <v>211004</v>
       </c>
       <c r="B66" t="str">
         <v>General Surgery</v>
@@ -1713,7 +1713,7 @@
         <v>20/10/2025</v>
       </c>
       <c r="D66" t="str">
-        <v>11:17:22</v>
+        <v>11:17:33</v>
       </c>
       <c r="E66" t="str">
         <v>Manual</v>
@@ -1724,7 +1724,7 @@
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>211004</v>
+        <v>201819</v>
       </c>
       <c r="B67" t="str">
         <v>General Surgery</v>
@@ -1733,7 +1733,7 @@
         <v>20/10/2025</v>
       </c>
       <c r="D67" t="str">
-        <v>11:17:33</v>
+        <v>11:17:41</v>
       </c>
       <c r="E67" t="str">
         <v>Manual</v>
@@ -1744,7 +1744,7 @@
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>201819</v>
+        <v>201065</v>
       </c>
       <c r="B68" t="str">
         <v>General Surgery</v>
@@ -1753,7 +1753,7 @@
         <v>20/10/2025</v>
       </c>
       <c r="D68" t="str">
-        <v>11:17:41</v>
+        <v>11:17:52</v>
       </c>
       <c r="E68" t="str">
         <v>Manual</v>
@@ -1764,7 +1764,7 @@
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>201065</v>
+        <v>201218</v>
       </c>
       <c r="B69" t="str">
         <v>General Surgery</v>
@@ -1773,7 +1773,7 @@
         <v>20/10/2025</v>
       </c>
       <c r="D69" t="str">
-        <v>11:17:52</v>
+        <v>11:17:59</v>
       </c>
       <c r="E69" t="str">
         <v>Manual</v>
@@ -1784,7 +1784,7 @@
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>201218</v>
+        <v>200999</v>
       </c>
       <c r="B70" t="str">
         <v>General Surgery</v>
@@ -1793,7 +1793,7 @@
         <v>20/10/2025</v>
       </c>
       <c r="D70" t="str">
-        <v>11:17:59</v>
+        <v>11:18:06</v>
       </c>
       <c r="E70" t="str">
         <v>Manual</v>
@@ -1804,7 +1804,7 @@
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>200999</v>
+        <v>201495</v>
       </c>
       <c r="B71" t="str">
         <v>General Surgery</v>
@@ -1813,7 +1813,7 @@
         <v>20/10/2025</v>
       </c>
       <c r="D71" t="str">
-        <v>11:18:06</v>
+        <v>11:18:14</v>
       </c>
       <c r="E71" t="str">
         <v>Manual</v>
@@ -1824,7 +1824,7 @@
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>201495</v>
+        <v>201632</v>
       </c>
       <c r="B72" t="str">
         <v>General Surgery</v>
@@ -1833,7 +1833,7 @@
         <v>20/10/2025</v>
       </c>
       <c r="D72" t="str">
-        <v>11:18:14</v>
+        <v>11:18:24</v>
       </c>
       <c r="E72" t="str">
         <v>Manual</v>
@@ -1844,7 +1844,7 @@
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>201632</v>
+        <v>200858</v>
       </c>
       <c r="B73" t="str">
         <v>General Surgery</v>
@@ -1853,7 +1853,7 @@
         <v>20/10/2025</v>
       </c>
       <c r="D73" t="str">
-        <v>11:18:24</v>
+        <v>11:18:33</v>
       </c>
       <c r="E73" t="str">
         <v>Manual</v>
@@ -1864,7 +1864,7 @@
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>200858</v>
+        <v>200824</v>
       </c>
       <c r="B74" t="str">
         <v>General Surgery</v>
@@ -1873,7 +1873,7 @@
         <v>20/10/2025</v>
       </c>
       <c r="D74" t="str">
-        <v>11:18:33</v>
+        <v>11:18:41</v>
       </c>
       <c r="E74" t="str">
         <v>Manual</v>
@@ -1884,7 +1884,7 @@
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>200824</v>
+        <v>200904</v>
       </c>
       <c r="B75" t="str">
         <v>General Surgery</v>
@@ -1893,7 +1893,7 @@
         <v>20/10/2025</v>
       </c>
       <c r="D75" t="str">
-        <v>11:18:41</v>
+        <v>11:18:49</v>
       </c>
       <c r="E75" t="str">
         <v>Manual</v>
@@ -1904,7 +1904,7 @@
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>200904</v>
+        <v>200914</v>
       </c>
       <c r="B76" t="str">
         <v>General Surgery</v>
@@ -1913,7 +1913,7 @@
         <v>20/10/2025</v>
       </c>
       <c r="D76" t="str">
-        <v>11:18:49</v>
+        <v>11:18:56</v>
       </c>
       <c r="E76" t="str">
         <v>Manual</v>
@@ -1924,7 +1924,7 @@
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v>200914</v>
+        <v>201638</v>
       </c>
       <c r="B77" t="str">
         <v>General Surgery</v>
@@ -1933,7 +1933,7 @@
         <v>20/10/2025</v>
       </c>
       <c r="D77" t="str">
-        <v>11:18:56</v>
+        <v>11:19:06</v>
       </c>
       <c r="E77" t="str">
         <v>Manual</v>
@@ -1944,7 +1944,7 @@
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v>201638</v>
+        <v>200869</v>
       </c>
       <c r="B78" t="str">
         <v>General Surgery</v>
@@ -1953,7 +1953,7 @@
         <v>20/10/2025</v>
       </c>
       <c r="D78" t="str">
-        <v>11:19:06</v>
+        <v>11:19:15</v>
       </c>
       <c r="E78" t="str">
         <v>Manual</v>
@@ -1964,7 +1964,7 @@
     </row>
     <row r="79">
       <c r="A79" t="str">
-        <v>200869</v>
+        <v>201197</v>
       </c>
       <c r="B79" t="str">
         <v>General Surgery</v>
@@ -1973,7 +1973,7 @@
         <v>20/10/2025</v>
       </c>
       <c r="D79" t="str">
-        <v>11:19:15</v>
+        <v>11:19:31</v>
       </c>
       <c r="E79" t="str">
         <v>Manual</v>
@@ -1984,7 +1984,7 @@
     </row>
     <row r="80">
       <c r="A80" t="str">
-        <v>201197</v>
+        <v>191480</v>
       </c>
       <c r="B80" t="str">
         <v>General Surgery</v>
@@ -1993,7 +1993,7 @@
         <v>20/10/2025</v>
       </c>
       <c r="D80" t="str">
-        <v>11:19:31</v>
+        <v>11:19:50</v>
       </c>
       <c r="E80" t="str">
         <v>Manual</v>
@@ -2004,7 +2004,7 @@
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>191480</v>
+        <v>191375</v>
       </c>
       <c r="B81" t="str">
         <v>General Surgery</v>
@@ -2013,7 +2013,7 @@
         <v>20/10/2025</v>
       </c>
       <c r="D81" t="str">
-        <v>11:19:50</v>
+        <v>11:20:01</v>
       </c>
       <c r="E81" t="str">
         <v>Manual</v>
@@ -2024,7 +2024,7 @@
     </row>
     <row r="82">
       <c r="A82" t="str">
-        <v>191375</v>
+        <v>200897</v>
       </c>
       <c r="B82" t="str">
         <v>General Surgery</v>
@@ -2033,7 +2033,7 @@
         <v>20/10/2025</v>
       </c>
       <c r="D82" t="str">
-        <v>11:20:01</v>
+        <v>11:20:17</v>
       </c>
       <c r="E82" t="str">
         <v>Manual</v>
@@ -2044,7 +2044,7 @@
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v>200897</v>
+        <v>200958</v>
       </c>
       <c r="B83" t="str">
         <v>General Surgery</v>
@@ -2053,7 +2053,7 @@
         <v>20/10/2025</v>
       </c>
       <c r="D83" t="str">
-        <v>11:20:17</v>
+        <v>11:22:35</v>
       </c>
       <c r="E83" t="str">
         <v>Manual</v>
@@ -2064,7 +2064,7 @@
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v>200958</v>
+        <v>201328</v>
       </c>
       <c r="B84" t="str">
         <v>General Surgery</v>
@@ -2073,7 +2073,7 @@
         <v>20/10/2025</v>
       </c>
       <c r="D84" t="str">
-        <v>11:22:35</v>
+        <v>11:23:16</v>
       </c>
       <c r="E84" t="str">
         <v>Manual</v>
@@ -2084,7 +2084,7 @@
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v>201328</v>
+        <v>201252</v>
       </c>
       <c r="B85" t="str">
         <v>General Surgery</v>
@@ -2093,7 +2093,7 @@
         <v>20/10/2025</v>
       </c>
       <c r="D85" t="str">
-        <v>11:23:16</v>
+        <v>11:23:35</v>
       </c>
       <c r="E85" t="str">
         <v>Manual</v>
@@ -2104,7 +2104,7 @@
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>201252</v>
+        <v>201253</v>
       </c>
       <c r="B86" t="str">
         <v>General Surgery</v>
@@ -2113,7 +2113,7 @@
         <v>20/10/2025</v>
       </c>
       <c r="D86" t="str">
-        <v>11:23:35</v>
+        <v>11:23:48</v>
       </c>
       <c r="E86" t="str">
         <v>Manual</v>
@@ -2124,7 +2124,7 @@
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>201253</v>
+        <v>201023</v>
       </c>
       <c r="B87" t="str">
         <v>General Surgery</v>
@@ -2133,7 +2133,7 @@
         <v>20/10/2025</v>
       </c>
       <c r="D87" t="str">
-        <v>11:23:48</v>
+        <v>11:23:58</v>
       </c>
       <c r="E87" t="str">
         <v>Manual</v>
@@ -2144,7 +2144,7 @@
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>201023</v>
+        <v>211137</v>
       </c>
       <c r="B88" t="str">
         <v>General Surgery</v>
@@ -2153,7 +2153,7 @@
         <v>20/10/2025</v>
       </c>
       <c r="D88" t="str">
-        <v>11:23:58</v>
+        <v>11:24:11</v>
       </c>
       <c r="E88" t="str">
         <v>Manual</v>
@@ -2164,7 +2164,7 @@
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v>211137</v>
+        <v>211189</v>
       </c>
       <c r="B89" t="str">
         <v>General Surgery</v>
@@ -2173,7 +2173,7 @@
         <v>20/10/2025</v>
       </c>
       <c r="D89" t="str">
-        <v>11:24:11</v>
+        <v>11:25:03</v>
       </c>
       <c r="E89" t="str">
         <v>Manual</v>
@@ -2184,7 +2184,7 @@
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v>211189</v>
+        <v>201838</v>
       </c>
       <c r="B90" t="str">
         <v>General Surgery</v>
@@ -2193,7 +2193,7 @@
         <v>20/10/2025</v>
       </c>
       <c r="D90" t="str">
-        <v>11:25:03</v>
+        <v>11:25:21</v>
       </c>
       <c r="E90" t="str">
         <v>Manual</v>
@@ -2204,7 +2204,7 @@
     </row>
     <row r="91">
       <c r="A91" t="str">
-        <v>201838</v>
+        <v>202022</v>
       </c>
       <c r="B91" t="str">
         <v>General Surgery</v>
@@ -2213,7 +2213,7 @@
         <v>20/10/2025</v>
       </c>
       <c r="D91" t="str">
-        <v>11:25:21</v>
+        <v>11:25:46</v>
       </c>
       <c r="E91" t="str">
         <v>Manual</v>
@@ -2224,7 +2224,7 @@
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v>202022</v>
+        <v>191055</v>
       </c>
       <c r="B92" t="str">
         <v>General Surgery</v>
@@ -2233,7 +2233,7 @@
         <v>20/10/2025</v>
       </c>
       <c r="D92" t="str">
-        <v>11:25:46</v>
+        <v>11:26:03</v>
       </c>
       <c r="E92" t="str">
         <v>Manual</v>
@@ -2244,7 +2244,7 @@
     </row>
     <row r="93">
       <c r="A93" t="str">
-        <v>191055</v>
+        <v>211210</v>
       </c>
       <c r="B93" t="str">
         <v>General Surgery</v>
@@ -2253,7 +2253,7 @@
         <v>20/10/2025</v>
       </c>
       <c r="D93" t="str">
-        <v>11:26:03</v>
+        <v>11:26:22</v>
       </c>
       <c r="E93" t="str">
         <v>Manual</v>
@@ -2264,7 +2264,7 @@
     </row>
     <row r="94">
       <c r="A94" t="str">
-        <v>211210</v>
+        <v>211169</v>
       </c>
       <c r="B94" t="str">
         <v>General Surgery</v>
@@ -2273,7 +2273,7 @@
         <v>20/10/2025</v>
       </c>
       <c r="D94" t="str">
-        <v>11:26:22</v>
+        <v>11:26:41</v>
       </c>
       <c r="E94" t="str">
         <v>Manual</v>
@@ -2284,7 +2284,7 @@
     </row>
     <row r="95">
       <c r="A95" t="str">
-        <v>211169</v>
+        <v>211246</v>
       </c>
       <c r="B95" t="str">
         <v>General Surgery</v>
@@ -2293,7 +2293,7 @@
         <v>20/10/2025</v>
       </c>
       <c r="D95" t="str">
-        <v>11:26:41</v>
+        <v>11:28:24</v>
       </c>
       <c r="E95" t="str">
         <v>Manual</v>
@@ -2304,7 +2304,7 @@
     </row>
     <row r="96">
       <c r="A96" t="str">
-        <v>211246</v>
+        <v>211217</v>
       </c>
       <c r="B96" t="str">
         <v>General Surgery</v>
@@ -2313,7 +2313,7 @@
         <v>20/10/2025</v>
       </c>
       <c r="D96" t="str">
-        <v>11:28:24</v>
+        <v>11:29:25</v>
       </c>
       <c r="E96" t="str">
         <v>Manual</v>
@@ -2324,7 +2324,7 @@
     </row>
     <row r="97">
       <c r="A97" t="str">
-        <v>211217</v>
+        <v>201823</v>
       </c>
       <c r="B97" t="str">
         <v>General Surgery</v>
@@ -2333,7 +2333,7 @@
         <v>20/10/2025</v>
       </c>
       <c r="D97" t="str">
-        <v>11:29:25</v>
+        <v>11:30:03</v>
       </c>
       <c r="E97" t="str">
         <v>Manual</v>
@@ -2344,7 +2344,7 @@
     </row>
     <row r="98">
       <c r="A98" t="str">
-        <v>201823</v>
+        <v>200943</v>
       </c>
       <c r="B98" t="str">
         <v>General Surgery</v>
@@ -2353,7 +2353,7 @@
         <v>20/10/2025</v>
       </c>
       <c r="D98" t="str">
-        <v>11:30:03</v>
+        <v>11:30:22</v>
       </c>
       <c r="E98" t="str">
         <v>Manual</v>
@@ -2364,7 +2364,7 @@
     </row>
     <row r="99">
       <c r="A99" t="str">
-        <v>200943</v>
+        <v>201237</v>
       </c>
       <c r="B99" t="str">
         <v>General Surgery</v>
@@ -2373,7 +2373,7 @@
         <v>20/10/2025</v>
       </c>
       <c r="D99" t="str">
-        <v>11:30:22</v>
+        <v>11:31:10</v>
       </c>
       <c r="E99" t="str">
         <v>Manual</v>
@@ -2384,7 +2384,7 @@
     </row>
     <row r="100">
       <c r="A100" t="str">
-        <v>201237</v>
+        <v>200928</v>
       </c>
       <c r="B100" t="str">
         <v>General Surgery</v>
@@ -2393,38 +2393,18 @@
         <v>20/10/2025</v>
       </c>
       <c r="D100" t="str">
-        <v>11:31:10</v>
+        <v>11:31:27</v>
       </c>
       <c r="E100" t="str">
         <v>Manual</v>
       </c>
       <c r="F100" t="str">
-        <v>dnasr281@gmail.com</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="str">
-        <v>200928</v>
-      </c>
-      <c r="B101" t="str">
-        <v>General Surgery</v>
-      </c>
-      <c r="C101" t="str">
-        <v>20/10/2025</v>
-      </c>
-      <c r="D101" t="str">
-        <v>11:31:27</v>
-      </c>
-      <c r="E101" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F101" t="str">
         <v>dnasr281@gmail.com</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F101"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F100"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>